<commit_message>
add CS programs: TUM_DATA_ENG TUBERLIN_CS FU_DATA RWTH_DATA_SCIENCE
</commit_message>
<xml_diff>
--- a/database/ChemicalEngineering/CME_Course_database.xlsx
+++ b/database/ChemicalEngineering/CME_Course_database.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ChemicalEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476BB392-DCC6-432F-8F19-49DC470F87BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AEF616-E101-4397-B0D3-F3389D6142F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
   <sheets>
-    <sheet name="All_ME_Courses" sheetId="1" r:id="rId1"/>
+    <sheet name="All_CME_Courses" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -766,7 +766,7 @@
   <dimension ref="A1:W424"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>

</xml_diff>